<commit_message>
edit for bracket invoice
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/brackets_invoice_summary.xlsx
+++ b/application/controllers/excel-templates/brackets_invoice_summary.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-aws\application\controllers\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-dev\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -53,9 +53,6 @@
     <t>No. Of Units</t>
   </si>
   <si>
-    <t>Unit Price</t>
-  </si>
-  <si>
     <t>Tax Rate %</t>
   </si>
   <si>
@@ -119,15 +116,6 @@
     <t>{invoice:total}</t>
   </si>
   <si>
-    <t>{invoice:19_24_total}</t>
-  </si>
-  <si>
-    <t>{invoice:26_32_total}</t>
-  </si>
-  <si>
-    <t>{invoice:36_42_total}</t>
-  </si>
-  <si>
     <t>{invoice:tax_rate}</t>
   </si>
   <si>
@@ -162,6 +150,18 @@
   </si>
   <si>
     <t>S. N.</t>
+  </si>
+  <si>
+    <t>{invoice:_19_24_total}</t>
+  </si>
+  <si>
+    <t>{invoice:_26_32_total}</t>
+  </si>
+  <si>
+    <t>{invoice:_36_42_total}</t>
+  </si>
+  <si>
+    <t>Basic Price</t>
   </si>
 </sst>
 </file>
@@ -578,7 +578,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -651,9 +651,6 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -708,6 +705,48 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -777,47 +816,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -842,9 +848,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>349250</xdr:colOff>
+      <xdr:colOff>330200</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
+      <xdr:rowOff>79375</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="609600" cy="561975"/>
     <xdr:pic>
@@ -862,7 +868,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7988300" y="298450"/>
+          <a:off x="5826125" y="269875"/>
           <a:ext cx="609600" cy="561975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1140,16 +1146,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="2"/>
+    <col min="2" max="2" width="5.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="8.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="29.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" style="2" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="14.42578125" style="2"/>
@@ -1157,7 +1163,7 @@
     <col min="9" max="9" width="7.28515625" style="2" customWidth="1"/>
     <col min="10" max="10" width="10" style="2" customWidth="1"/>
     <col min="11" max="11" width="8.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="7.28515625" style="2" customWidth="1"/>
     <col min="13" max="16384" width="14.42578125" style="2"/>
   </cols>
   <sheetData>
@@ -1178,16 +1184,16 @@
     <row r="2" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
-      <c r="F2" s="7" t="s">
-        <v>25</v>
-      </c>
+      <c r="F2" s="7"/>
       <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="H2" s="81" t="s">
+        <v>24</v>
+      </c>
       <c r="I2" s="6"/>
       <c r="J2" s="8"/>
       <c r="K2" s="9"/>
@@ -1201,11 +1207,11 @@
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="13"/>
-      <c r="F3" s="14" t="s">
-        <v>26</v>
-      </c>
+      <c r="F3" s="14"/>
       <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
+      <c r="H3" s="82" t="s">
+        <v>25</v>
+      </c>
       <c r="I3" s="13"/>
       <c r="J3" s="15"/>
       <c r="K3" s="16"/>
@@ -1296,7 +1302,7 @@
       </c>
       <c r="C9" s="21"/>
       <c r="D9" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -1307,285 +1313,279 @@
       <c r="K9" s="16"/>
       <c r="L9" s="17"/>
     </row>
-    <row r="10" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="24"/>
       <c r="C10" s="25"/>
-      <c r="D10" s="26" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="30"/>
+      <c r="D10" s="83" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="29"/>
     </row>
     <row r="11" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="31"/>
-      <c r="B11" s="32" t="s">
+      <c r="A11" s="30"/>
+      <c r="B11" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="62" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="63"/>
+      <c r="E11" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="49" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="50"/>
-      <c r="E11" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="33" t="s">
+      <c r="H11" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="I11" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="33" t="s">
+      <c r="J11" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="49" t="s">
+      <c r="K11" s="64"/>
+      <c r="L11" s="65"/>
+    </row>
+    <row r="12" spans="1:12" ht="51" x14ac:dyDescent="0.25">
+      <c r="A12" s="30"/>
+      <c r="B12" s="33">
+        <v>1</v>
+      </c>
+      <c r="C12" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="51"/>
-      <c r="L11" s="52"/>
-    </row>
-    <row r="12" spans="1:12" ht="51" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
-      <c r="B12" s="34">
-        <v>1</v>
-      </c>
-      <c r="C12" s="53" t="s">
+      <c r="D12" s="66"/>
+      <c r="E12" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="53"/>
-      <c r="E12" s="35" t="s">
+      <c r="F12" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="I12" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" s="67"/>
+      <c r="L12" s="68"/>
+    </row>
+    <row r="13" spans="1:12" ht="51" x14ac:dyDescent="0.25">
+      <c r="A13" s="30"/>
+      <c r="B13" s="33">
+        <v>2</v>
+      </c>
+      <c r="C13" s="69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="69"/>
+      <c r="E13" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="36" t="s">
+      <c r="F13" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" s="42" t="s">
+        <v>30</v>
+      </c>
+      <c r="I13" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="J13" s="70" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="K12" s="54"/>
-      <c r="L12" s="55"/>
-    </row>
-    <row r="13" spans="1:12" ht="51" x14ac:dyDescent="0.25">
-      <c r="A13" s="31"/>
-      <c r="B13" s="34">
-        <v>2</v>
-      </c>
-      <c r="C13" s="56" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="56"/>
-      <c r="E13" s="35" t="s">
+      <c r="K13" s="70"/>
+      <c r="L13" s="71"/>
+    </row>
+    <row r="14" spans="1:12" ht="51" x14ac:dyDescent="0.25">
+      <c r="A14" s="30"/>
+      <c r="B14" s="36">
+        <v>3</v>
+      </c>
+      <c r="C14" s="72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="72"/>
+      <c r="E14" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="36" t="s">
+      <c r="F14" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="I14" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="J14" s="70" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="43" t="s">
-        <v>34</v>
-      </c>
-      <c r="I13" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="K13" s="57"/>
-      <c r="L13" s="58"/>
-    </row>
-    <row r="14" spans="1:12" ht="51" x14ac:dyDescent="0.25">
-      <c r="A14" s="31"/>
-      <c r="B14" s="37">
-        <v>3</v>
-      </c>
-      <c r="C14" s="59" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="59"/>
-      <c r="E14" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="F14" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="G14" s="39" t="s">
-        <v>40</v>
-      </c>
-      <c r="H14" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="I14" s="40" t="s">
-        <v>37</v>
-      </c>
-      <c r="J14" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="K14" s="57"/>
-      <c r="L14" s="58"/>
+      <c r="K14" s="70"/>
+      <c r="L14" s="71"/>
     </row>
     <row r="15" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="31"/>
-      <c r="B15" s="41"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="40"/>
       <c r="C15" s="16"/>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
-      <c r="F15" s="42" t="s">
-        <v>17</v>
+      <c r="F15" s="41" t="s">
+        <v>16</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
       <c r="I15" s="16"/>
-      <c r="J15" s="60" t="s">
-        <v>30</v>
-      </c>
-      <c r="K15" s="60"/>
-      <c r="L15" s="61"/>
+      <c r="J15" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="K15" s="73"/>
+      <c r="L15" s="74"/>
     </row>
     <row r="16" spans="1:12" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="31"/>
-      <c r="B16" s="62" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" s="63"/>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
-      <c r="H16" s="63"/>
-      <c r="I16" s="63"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="63"/>
-      <c r="L16" s="64"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="75" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="76"/>
+      <c r="K16" s="76"/>
+      <c r="L16" s="77"/>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="31"/>
-      <c r="B17" s="79"/>
-      <c r="C17" s="80"/>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80"/>
-      <c r="H17" s="80"/>
-      <c r="I17" s="80"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="80"/>
-      <c r="L17" s="81"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="45"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="46"/>
     </row>
     <row r="18" spans="1:12" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="31"/>
-      <c r="B18" s="65" t="s">
+      <c r="A18" s="30"/>
+      <c r="B18" s="78" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="79"/>
+      <c r="D18" s="79"/>
+      <c r="E18" s="79"/>
+      <c r="F18" s="79"/>
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="80"/>
+    </row>
+    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="30"/>
+      <c r="B19" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-      <c r="G18" s="66"/>
-      <c r="H18" s="66"/>
-      <c r="I18" s="66"/>
-      <c r="J18" s="66"/>
-      <c r="K18" s="66"/>
-      <c r="L18" s="67"/>
-    </row>
-    <row r="19" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="31"/>
-      <c r="B19" s="45" t="s">
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="61"/>
+    </row>
+    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="30"/>
+      <c r="B20" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="47" t="s">
-        <v>0</v>
-      </c>
-      <c r="F19" s="46"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46"/>
-      <c r="J19" s="46"/>
-      <c r="K19" s="46"/>
-      <c r="L19" s="48"/>
-    </row>
-    <row r="20" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="31"/>
-      <c r="B20" s="68" t="s">
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="49">
+        <v>102405500277</v>
+      </c>
+      <c r="F20" s="50"/>
+      <c r="G20" s="50"/>
+      <c r="H20" s="50"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="50"/>
+      <c r="L20" s="51"/>
+    </row>
+    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="30"/>
+      <c r="B21" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="70">
-        <v>102405500277</v>
-      </c>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="71"/>
-      <c r="J20" s="71"/>
-      <c r="K20" s="71"/>
-      <c r="L20" s="72"/>
-    </row>
-    <row r="21" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="31"/>
-      <c r="B21" s="68" t="s">
+      <c r="C21" s="48"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="73" t="s">
+      <c r="F21" s="48"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="48"/>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="53"/>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="69"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="74"/>
-    </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="75" t="s">
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="C22" s="76"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="77" t="s">
-        <v>24</v>
-      </c>
-      <c r="F22" s="76"/>
-      <c r="G22" s="76"/>
-      <c r="H22" s="76"/>
-      <c r="I22" s="76"/>
-      <c r="J22" s="76"/>
-      <c r="K22" s="76"/>
-      <c r="L22" s="78"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55"/>
+      <c r="H22" s="55"/>
+      <c r="I22" s="55"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="55"/>
+      <c r="L22" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:L20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:L21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:L22"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="E19:L19"/>
     <mergeCell ref="C11:D11"/>
@@ -1599,6 +1599,12 @@
     <mergeCell ref="J15:L15"/>
     <mergeCell ref="B16:L16"/>
     <mergeCell ref="B18:L18"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:L20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:L21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:L22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>